<commit_message>
Updates for Stevens Player Swap
</commit_message>
<xml_diff>
--- a/mchc/2022-23-MCHC-ASG-Rosters.xlsx
+++ b/mchc/2022-23-MCHC-ASG-Rosters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/methockey/mchc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{CAB1F0CE-35A3-4CBE-A315-5895E50D9A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B02F61EC-2453-4017-8672-6FC35B04E597}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{CAB1F0CE-35A3-4CBE-A315-5895E50D9A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3143D47B-5B34-4B77-8884-95F75E508623}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BAD27827-DCC5-4A9F-885D-CA33DE65F59B}"/>
   </bookViews>
@@ -119,9 +119,6 @@
     <t>Matthias</t>
   </si>
   <si>
-    <t>Maciej</t>
-  </si>
-  <si>
     <t>Shea</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>Paltauf</t>
   </si>
   <si>
-    <t>Kowalczyk</t>
-  </si>
-  <si>
     <t>Barthold</t>
   </si>
   <si>
@@ -368,9 +362,6 @@
     <t>Newtown HS</t>
   </si>
   <si>
-    <t>St. Peter's Prep</t>
-  </si>
-  <si>
     <t>Toms River HS North</t>
   </si>
   <si>
@@ -464,9 +455,6 @@
     <t>Newtown, CT</t>
   </si>
   <si>
-    <t>Bayonne, NJ</t>
-  </si>
-  <si>
     <t>Toms River, NJ</t>
   </si>
   <si>
@@ -486,6 +474,18 @@
   </si>
   <si>
     <t>Danbury, CT</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Canales</t>
+  </si>
+  <si>
+    <t>St. Rose HS</t>
+  </si>
+  <si>
+    <t>Neptune, NJ</t>
   </si>
 </sst>
 </file>
@@ -643,6 +643,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -944,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905C1F3D-B9AA-423C-A872-B03F480BD014}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -983,28 +987,28 @@
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="I2" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1015,10 +1019,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E3" s="2">
         <v>11</v>
@@ -1031,16 +1035,16 @@
         <v>20</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1051,10 +1055,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E4" s="2">
         <v>7</v>
@@ -1067,16 +1071,16 @@
         <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1087,10 +1091,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E5" s="2">
         <v>10</v>
@@ -1103,16 +1107,16 @@
         <v>23</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1123,10 +1127,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E6" s="2">
         <v>7</v>
@@ -1139,16 +1143,16 @@
         <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1159,10 +1163,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2">
         <v>17</v>
@@ -1175,16 +1179,16 @@
         <v>28</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1195,10 +1199,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -1211,16 +1215,16 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1231,10 +1235,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E9" s="2">
         <v>20</v>
@@ -1247,16 +1251,16 @@
         <v>30</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1267,10 +1271,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E10" s="2">
         <v>7</v>
@@ -1283,16 +1287,16 @@
         <v>14</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1303,10 +1307,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E11" s="2">
         <v>9</v>
@@ -1319,16 +1323,16 @@
         <v>20</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1339,10 +1343,10 @@
         <v>13</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E12" s="2">
         <v>9</v>
@@ -1355,16 +1359,16 @@
         <v>25</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1375,10 +1379,10 @@
         <v>14</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E13" s="2">
         <v>0</v>
@@ -1391,16 +1395,16 @@
         <v>4</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1411,10 +1415,10 @@
         <v>15</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E14" s="2">
         <v>10</v>
@@ -1427,16 +1431,16 @@
         <v>21</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1447,10 +1451,10 @@
         <v>16</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E15" s="2">
         <v>16</v>
@@ -1463,16 +1467,16 @@
         <v>37</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1483,10 +1487,10 @@
         <v>17</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E16" s="2">
         <v>19</v>
@@ -1499,16 +1503,16 @@
         <v>26</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1519,10 +1523,10 @@
         <v>18</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E17" s="2">
         <v>7</v>
@@ -1535,16 +1539,16 @@
         <v>26</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1569,26 +1573,26 @@
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="G19" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>73</v>
-      </c>
       <c r="H19" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J19" s="11"/>
       <c r="K19" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1599,10 +1603,10 @@
         <v>20</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E20" s="2">
         <v>2.37</v>
@@ -1614,16 +1618,16 @@
         <v>709</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1634,10 +1638,10 @@
         <v>12</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E21" s="2">
         <v>3.53</v>
@@ -1649,16 +1653,16 @@
         <v>663</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1698,28 +1702,28 @@
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="G24" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="H24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="I24" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1730,10 +1734,10 @@
         <v>21</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E25" s="2">
         <v>4</v>
@@ -1742,20 +1746,20 @@
         <v>14</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" ref="G25:G39" si="1">E25+F25</f>
+        <f t="shared" ref="G25:G38" si="1">E25+F25</f>
         <v>18</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1766,10 +1770,10 @@
         <v>22</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E26" s="2">
         <v>3</v>
@@ -1782,16 +1786,16 @@
         <v>9</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1802,10 +1806,10 @@
         <v>18</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E27" s="2">
         <v>3</v>
@@ -1818,16 +1822,16 @@
         <v>20</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1838,10 +1842,10 @@
         <v>23</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E28" s="2">
         <v>4</v>
@@ -1854,16 +1858,16 @@
         <v>14</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1874,10 +1878,10 @@
         <v>8</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E29" s="2">
         <v>9</v>
@@ -1890,16 +1894,16 @@
         <v>19</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1910,10 +1914,10 @@
         <v>24</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E30" s="2">
         <v>7</v>
@@ -1926,16 +1930,16 @@
         <v>13</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1946,10 +1950,10 @@
         <v>25</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E31" s="2">
         <v>11</v>
@@ -1962,16 +1966,16 @@
         <v>22</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1982,10 +1986,10 @@
         <v>26</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E32" s="2">
         <v>6</v>
@@ -1998,124 +2002,124 @@
         <v>14</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E33" s="2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F33" s="2">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E34" s="2">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F34" s="2">
         <v>8</v>
       </c>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E35" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F35" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>79</v>
+        <v>22</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -2123,143 +2127,142 @@
         <v>19</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E36" s="2">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F36" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>76</v>
+        <v>12</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E37" s="2">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F37" s="2">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I37" s="7" t="s">
         <v>84</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E38" s="2">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F38" s="2">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>30</v>
+        <v>146</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>62</v>
+        <v>147</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E39" s="2">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F39" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G39" s="2">
-        <f t="shared" si="1"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -2284,26 +2287,26 @@
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E41" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="G41" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G41" s="6" t="s">
-        <v>73</v>
-      </c>
       <c r="H41" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J41" s="11"/>
       <c r="K41" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -2311,13 +2314,13 @@
         <v>39</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E42" s="2">
         <v>3.06</v>
@@ -2329,16 +2332,16 @@
         <v>923</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -2346,13 +2349,13 @@
         <v>33</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E43" s="2">
         <v>4.78</v>
@@ -2364,16 +2367,16 @@
         <v>1067</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>